<commit_message>
Solucionando fallas del pull
</commit_message>
<xml_diff>
--- a/retos/asistente.xlsx
+++ b/retos/asistente.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jj\scholar\aUsa\c2\retos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\JJ\scholar\aUsa\c02\pgm\retos\retos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F7AEAF7-3C14-4AFB-8490-7560188D1121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{E53ACBE7-E907-49D3-BDDD-BEC47C3F14EE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="reemp" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Edad &lt; 45 Edad ≥ 45</t>
   </si>
@@ -66,12 +65,15 @@
   </si>
   <si>
     <t>Alto</t>
+  </si>
+  <si>
+    <t>K:\JJ\scholar\aUsa\c02\pgm\retos\retos\tut\ciclosJDBurbano\src\ciclosjdburbano\CiclosJDBurbano.java</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -448,10 +450,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE69AD33-CAE6-4477-9034-CAB1A195711E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -520,13 +522,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB1F875-1C48-4BD3-BBBE-459C6897177D}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="95" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="str">
+        <f>+REPLACE(A1,1,100,"/")</f>
+        <v>/</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reto 2 con método agregar OK
</commit_message>
<xml_diff>
--- a/retos/asistente.xlsx
+++ b/retos/asistente.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="reemp" sheetId="2" r:id="rId2"/>
+    <sheet name="reto2" sheetId="3" r:id="rId2"/>
+    <sheet name="reemp" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="27">
   <si>
     <t>Edad &lt; 45 Edad ≥ 45</t>
   </si>
@@ -68,13 +69,61 @@
   </si>
   <si>
     <t>K:\JJ\scholar\aUsa\c02\pgm\retos\retos\tut\ciclosJDBurbano\src\ciclosjdburbano\CiclosJDBurbano.java</t>
+  </si>
+  <si>
+    <t>listaProductos.put(</t>
+  </si>
+  <si>
+    <t>, new Producto(</t>
+  </si>
+  <si>
+    <t>Manzanas</t>
+  </si>
+  <si>
+    <t>Limones</t>
+  </si>
+  <si>
+    <t>Peras</t>
+  </si>
+  <si>
+    <t>Arandanos</t>
+  </si>
+  <si>
+    <t>Tomates</t>
+  </si>
+  <si>
+    <t>Fresas</t>
+  </si>
+  <si>
+    <t>Helado</t>
+  </si>
+  <si>
+    <t>Galletas</t>
+  </si>
+  <si>
+    <t>Chocolates</t>
+  </si>
+  <si>
+    <t>Jamon</t>
+  </si>
+  <si>
+    <t>));</t>
+  </si>
+  <si>
+    <t>, "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">.0, </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +145,13 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -105,7 +161,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -128,15 +184,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,9 +598,448 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="H11:J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="5">
+        <v>5000</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="6">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="str">
+        <f>+CONCATENATE(A1,B1,C1,D1,E1,F1,G1,H1,I1,J1,K1)</f>
+        <v>listaProductos.put(1, new Producto(1, "Manzanas", 5000.0, 25));</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="5">
+        <v>2300</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="6">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" ref="L2:L10" si="0">+CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2)</f>
+        <v>listaProductos.put(2, new Producto(2, "Limones", 2300.0, 15));</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="5">
+        <v>2700</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="6">
+        <v>33</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="0"/>
+        <v>listaProductos.put(3, new Producto(3, "Peras", 2700.0, 33));</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="5">
+        <v>9300</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="6">
+        <v>5</v>
+      </c>
+      <c r="K4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="0"/>
+        <v>listaProductos.put(4, new Producto(4, "Arandanos", 9300.0, 5));</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="5">
+        <v>2100</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="6">
+        <v>42</v>
+      </c>
+      <c r="K5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="0"/>
+        <v>listaProductos.put(5, new Producto(5, "Tomates", 2100.0, 42));</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="5">
+        <v>4100</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="6">
+        <v>3</v>
+      </c>
+      <c r="K6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="0"/>
+        <v>listaProductos.put(6, new Producto(6, "Fresas", 4100.0, 3));</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="5">
+        <v>4500</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="6">
+        <v>41</v>
+      </c>
+      <c r="K7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>listaProductos.put(7, new Producto(7, "Helado", 4500.0, 41));</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="5">
+        <v>500</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="6">
+        <v>8</v>
+      </c>
+      <c r="K8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v>listaProductos.put(8, new Producto(8, "Galletas", 500.0, 8));</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="5">
+        <v>3500</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="6">
+        <v>80</v>
+      </c>
+      <c r="K9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v>listaProductos.put(9, new Producto(9, "Chocolates", 3500.0, 80));</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="5">
+        <v>15000</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="6">
+        <v>10</v>
+      </c>
+      <c r="K10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v>listaProductos.put(10, new Producto(10, "Jamon", 15000.0, 10));</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H11" s="7">
+        <f t="shared" ref="H11:I11" si="1">SUM(H1:H10)</f>
+        <v>49000</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="7">
+        <f>SUM(J1:J10)</f>
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J12" s="7">
+        <f>13+J11</f>
+        <v>275</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Excel con casos de prueba
</commit_message>
<xml_diff>
--- a/retos/asistente.xlsx
+++ b/retos/asistente.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="reto2" sheetId="3" r:id="rId2"/>
-    <sheet name="reemp" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja2" sheetId="4" r:id="rId3"/>
+    <sheet name="reemp" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="46">
   <si>
     <t>Edad &lt; 45 Edad ≥ 45</t>
   </si>
@@ -117,6 +118,63 @@
   </si>
   <si>
     <t xml:space="preserve">.0, </t>
+  </si>
+  <si>
+    <t>ACT</t>
+  </si>
+  <si>
+    <t>7 Helado 65000 11</t>
+  </si>
+  <si>
+    <t>Helado Galletas 10950.0 1544600.0</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Jamon 500 10 </t>
+  </si>
+  <si>
+    <t>Arandanos Galletas 3450.0 869100.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 Papa 1500 10 </t>
+  </si>
+  <si>
+    <t>BOR</t>
+  </si>
+  <si>
+    <t>10 Jamon 15000 10</t>
+  </si>
+  <si>
+    <t>Arandanos Galletas 3777.8 864100.0</t>
+  </si>
+  <si>
+    <t>AGR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Peras 2700 33 </t>
+  </si>
+  <si>
+    <t>Jamon Galletas 5144.4 925000.0</t>
+  </si>
+  <si>
+    <t>15 Papa 1500 10</t>
+  </si>
+  <si>
+    <t>11 Melon 70 13</t>
+  </si>
+  <si>
+    <t>Jamon Melon 4460.9 1015010.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 Maiz 45000 12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 Maiz 70000 1 </t>
+  </si>
+  <si>
+    <t>Maiz Galletas 10818.2 1084100.0</t>
   </si>
 </sst>
 </file>
@@ -600,7 +658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="H11:J11"/>
     </sheetView>
   </sheetViews>
@@ -1037,6 +1095,138 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="str">
+        <f>+A1&amp;"  "&amp;B1&amp;"\t"&amp;C1&amp;"\t"&amp;E1&amp;"  "&amp;F1</f>
+        <v xml:space="preserve">ACT  7 Helado 65000 11\tHelado Galletas 10950.0 1544600.0\tERROR  </v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G3" si="0">+A2&amp;"  "&amp;B2&amp;"\t"&amp;C2&amp;"\t"&amp;E2&amp;"  "&amp;F2</f>
+        <v xml:space="preserve">ACT  10 Jamon 500 10 \tArandanos Galletas 3450.0 869100.0\tACT  15 Papa 1500 10 </v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">BOR  10 Jamon 15000 10\tArandanos Galletas 3777.8 864100.0\tAGR  3 Peras 2700 33 </v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" t="str">
+        <f>+A4&amp;"  "&amp;B4&amp;"\t"&amp;C4&amp;"\t\t"&amp;E4&amp;"  "&amp;F4</f>
+        <v>BOR  3 Peras 2700 33 \tJamon Galletas 5144.4 925000.0\t\tBOR  15 Papa 1500 10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="str">
+        <f>+A5&amp;"  "&amp;B5&amp;"\t"&amp;C5&amp;"\t\t"&amp;E5&amp;"  "&amp;F5</f>
+        <v xml:space="preserve">AGR  11 Melon 70 13\tJamon Melon 4460.9 1015010.0\t\tBOR  14 Maiz 45000 12 </v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" ref="G6" si="1">+A6&amp;"  "&amp;B6&amp;"\t"&amp;C6&amp;"\t\t"&amp;E6&amp;"  "&amp;F6</f>
+        <v xml:space="preserve">AGR  11 Maiz 70000 1 \tMaiz Galletas 10818.2 1084100.0\t\t  </v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>